<commit_message>
added hero card text support
changed to data table render
added some comments
noted hero bug with custom scheme (unfixed)
added card text of heroes (from bgg)
</commit_message>
<xml_diff>
--- a/support/results.xlsx
+++ b/support/results.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="179">
   <si>
     <t>Heroes</t>
   </si>
@@ -531,6 +531,27 @@
   </si>
   <si>
     <t>28|32</t>
+  </si>
+  <si>
+    <t>Organized crime-wave</t>
+  </si>
+  <si>
+    <t>Nick Fury</t>
+  </si>
+  <si>
+    <t>Avengers|Illuminati</t>
+  </si>
+  <si>
+    <t>Maggia Goons</t>
+  </si>
+  <si>
+    <t>Speed (R)|The Captain &amp; The Devil (SW2)|Goliath (CW)|Captain Marvel, Agent of SHIELD (R)|Totally Awesome Hulk (CH)</t>
+  </si>
+  <si>
+    <t>2|9</t>
+  </si>
+  <si>
+    <t>Goons sequenced into a twist once for 3 and once for 2. Lots of wounds and insufficient thinning as goons get twisted before you can beat them.</t>
   </si>
 </sst>
 </file>
@@ -871,10 +892,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K23"/>
+  <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1663,6 +1684,38 @@
         <v>170</v>
       </c>
     </row>
+    <row r="24" spans="1:11">
+      <c r="A24">
+        <v>2</v>
+      </c>
+      <c r="B24" t="s">
+        <v>172</v>
+      </c>
+      <c r="C24" t="s">
+        <v>173</v>
+      </c>
+      <c r="D24" t="s">
+        <v>174</v>
+      </c>
+      <c r="E24" t="s">
+        <v>175</v>
+      </c>
+      <c r="F24" t="s">
+        <v>176</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24" t="s">
+        <v>177</v>
+      </c>
+      <c r="I24" t="s">
+        <v>23</v>
+      </c>
+      <c r="K24" t="s">
+        <v>178</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
add export for tabletop simulator
add extra export format to tabletop simulator
</commit_message>
<xml_diff>
--- a/support/results.xlsx
+++ b/support/results.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="298">
   <si>
     <t>Heroes</t>
   </si>
@@ -894,6 +894,21 @@
   </si>
   <si>
     <t>70|36</t>
+  </si>
+  <si>
+    <t>Marauders|Shadow-X</t>
+  </si>
+  <si>
+    <t>Deadpool (B)|Slapstick (DP)|Bullseye (V)|Nerkkod, Breaker of Oceans (FI)|Thing (FF)</t>
+  </si>
+  <si>
+    <t>Hit the final tactic turn before likely lethal twist.</t>
+  </si>
+  <si>
+    <t>War Machine as extra hero</t>
+  </si>
+  <si>
+    <t>32|24</t>
   </si>
 </sst>
 </file>
@@ -1234,10 +1249,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K42"/>
+  <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="H43" sqref="H43"/>
+    <sheetView tabSelected="1" topLeftCell="D22" workbookViewId="0">
+      <selection activeCell="H44" sqref="H44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2643,6 +2658,41 @@
         <v>291</v>
       </c>
     </row>
+    <row r="43" spans="1:11">
+      <c r="A43">
+        <v>2</v>
+      </c>
+      <c r="B43" t="s">
+        <v>246</v>
+      </c>
+      <c r="C43" t="s">
+        <v>193</v>
+      </c>
+      <c r="D43" t="s">
+        <v>293</v>
+      </c>
+      <c r="E43" t="s">
+        <v>262</v>
+      </c>
+      <c r="F43" t="s">
+        <v>294</v>
+      </c>
+      <c r="G43">
+        <v>1</v>
+      </c>
+      <c r="H43" t="s">
+        <v>297</v>
+      </c>
+      <c r="I43" t="s">
+        <v>30</v>
+      </c>
+      <c r="J43" t="s">
+        <v>296</v>
+      </c>
+      <c r="K43" t="s">
+        <v>295</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
fix card text styles
fix card text styles
fix bug with set in text popup
</commit_message>
<xml_diff>
--- a/support/results.xlsx
+++ b/support/results.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="309">
   <si>
     <t>Heroes</t>
   </si>
@@ -924,6 +924,24 @@
   </si>
   <si>
     <t>SHIELD level was extremely strong in this one.</t>
+  </si>
+  <si>
+    <t>Mephisto</t>
+  </si>
+  <si>
+    <t>Underworld|Aspects of the Void</t>
+  </si>
+  <si>
+    <t>The Brood|Cape-Killers</t>
+  </si>
+  <si>
+    <t>Dr. Octopus (V)|Captain America (B)|Namora (WW)|Caiera (WW)|Invisible Woman (FF)</t>
+  </si>
+  <si>
+    <t>Lots of wounds, but also lots of ways to KO them (or the twists before they spawn wounds). Did get to 5 escaped villains.</t>
+  </si>
+  <si>
+    <t>17|33</t>
   </si>
 </sst>
 </file>
@@ -1264,10 +1282,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K44"/>
+  <dimension ref="A1:K45"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E16" workbookViewId="0">
-      <selection activeCell="K45" sqref="K45"/>
+      <selection activeCell="H46" sqref="H46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2740,6 +2758,38 @@
         <v>302</v>
       </c>
     </row>
+    <row r="45" spans="1:11">
+      <c r="A45">
+        <v>2</v>
+      </c>
+      <c r="B45" t="s">
+        <v>113</v>
+      </c>
+      <c r="C45" t="s">
+        <v>303</v>
+      </c>
+      <c r="D45" t="s">
+        <v>304</v>
+      </c>
+      <c r="E45" t="s">
+        <v>305</v>
+      </c>
+      <c r="F45" t="s">
+        <v>306</v>
+      </c>
+      <c r="G45">
+        <v>1</v>
+      </c>
+      <c r="H45" t="s">
+        <v>308</v>
+      </c>
+      <c r="I45" t="s">
+        <v>104</v>
+      </c>
+      <c r="K45" t="s">
+        <v>307</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>